<commit_message>
modied comprehension questions. corrected mixed up practice trials.
</commit_message>
<xml_diff>
--- a/html/resources/stimuli_tables/comprehension_questions.xlsx
+++ b/html/resources/stimuli_tables/comprehension_questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zsuzsa\HCCCL\experiment\computer_based_tasks\terkepesz_grid\TerKepEsz_Online\stimuli_tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zsuzsa\HCCCL\experiment\computer_based_tasks\terkepesz\terkepesz_encoding\TerKepEsz\stimuli_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6671A8F-81DB-44BF-90DF-7251AB753C13}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDDFC92-9487-40C8-A848-6106C5446A3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
   <si>
     <t>Question</t>
   </si>
@@ -78,21 +78,10 @@
     <t xml:space="preserve">Bizonyosodjon meg róla, hogy elég időt tud a vizsgálatra szánni. </t>
   </si>
   <si>
-    <t>Mely billentyű jelzi azokat a képeket, amelyek maradhatnak a galériában, a bemutatott helyen?</t>
-  </si>
-  <si>
     <t>D billentyű    F billentyű   J billentyű    K billentyű</t>
   </si>
   <si>
     <t>A helyes válasz: J billentyű.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Az első feladat nagyjából 25 percet vesz igénybe, közben két rövid szünettel. Ügyeljen, hogy ezek a szünetek ne legyenek 2 percnél hosszabbak. 
-A 'J' billentyűvel jelölje azokat a képeket, amelyek maradhatnak a galériában, a bemutatott helyen.
-Az 'F' billentyűvel jelölje a képeket, amelyek nem maradnak kiállítva a bemutatott helyen. </t>
-  </si>
-  <si>
-    <t>Mely billentyű jelzi azokat a képeket, amelyek nem maradhatnak a bemutatott helyen?</t>
   </si>
   <si>
     <t>A helyes válasz: F billentyű</t>
@@ -172,6 +161,20 @@
 A döntését így jelölje:
 Régi - F
 Új – J</t>
+  </si>
+  <si>
+    <t>Mely billentyű jelzi azokat a képeket, amelyeket beválogat a kiállításra a 'Kép' alfeladatban?</t>
+  </si>
+  <si>
+    <t>Mely billentyű jelzi azokat a képeket, amelyek nem maradhatnak a bemutatott helyen a 'Hely' alfeladatban?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 'J' billentyűvel jelölje azokat a képeket, amelyeket beválogat a kiállításra.
+Az 'F' billentyűvel jelölje a képeket, amelyeket nem válogat be a kiállításra. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 'J' billentyűvel jelölje azokat a képeket, amelyek maradhatnak a bemutatott helyen.
+Az 'F' billentyűvel jelölje a képeket, amelyek nem maradnak a bemutatott helyen. </t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -604,184 +607,184 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjusted comprehension questions for new version
</commit_message>
<xml_diff>
--- a/html/resources/stimuli_tables/comprehension_questions.xlsx
+++ b/html/resources/stimuli_tables/comprehension_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zsuzsa\HCCCL\experiment\computer_based_tasks\terkepesz\terkepesz_encoding\TerKepEsz\stimuli_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDDFC92-9487-40C8-A848-6106C5446A3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6001B64-3461-4106-95F4-DCB86802D78F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>Question</t>
   </si>
@@ -102,15 +102,6 @@
     <t xml:space="preserve">Kérjük, próbáljon meg a továbbiakban figyelni a képekre. </t>
   </si>
   <si>
-    <t>Mit gondol, ebben a körben milyen arányban tudott figyelni a képek helyére? Kérjük, válaszoljon őszintén. Válasza a vizsgálat bejefezésével járó jutalom (kredit, ajándékutalvány) értékét nem befolyásolja.</t>
-  </si>
-  <si>
-    <t>Kevesebb, mint 75%-ban tudott a képek helyszínére figyelni.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kérjük, próbáljon meg a továbbiakban figyelni a képek helyszínére. </t>
-  </si>
-  <si>
     <t>Hány másodperce lesz a döntésre egy-egy képről?</t>
   </si>
   <si>
@@ -120,19 +111,10 @@
     <t xml:space="preserve">A helyes válasz 4 mp. </t>
   </si>
   <si>
-    <t>Mit gondol, az első ‘Galéria berendezés’ feladatban mennyi olyan kép volt, amit nem nézett meg figyelmesen?</t>
-  </si>
-  <si>
-    <t>D: 0-10    F: 10-30    J: 30-50    K: több, mint 50</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
     <t>Köszönjük a választ.</t>
-  </si>
-  <si>
-    <t>Mit gondol, a második ‘Képfelismerés’ feladatban mennyi olyan kép volt, amit nem nézett meg figyelmesen?</t>
   </si>
   <si>
     <t>Hogy érzi, lelkiismeretesen, figyelmesen oldotta meg a feladatokat? Kérjük, válaszoljon őszintén. Válasza a vizsgálat bejefezésével járó jutalom (kredit, ajándékutalvány) értékét nem befolyásolja.</t>
@@ -175,6 +157,12 @@
   <si>
     <t xml:space="preserve">A 'J' billentyűvel jelölje azokat a képeket, amelyek maradhatnak a bemutatott helyen.
 Az 'F' billentyűvel jelölje a képeket, amelyek nem maradnak a bemutatott helyen. </t>
+  </si>
+  <si>
+    <t>Melyik billentyűvel jelölte a képeket, amelyek pontosan ugyanolyanok voltak, mint a megelőző Galériaberendezés feladatban?</t>
+  </si>
+  <si>
+    <t>Melyik billentyűvel jelölte azokat a képeket, amelyeket beválogatott a galériába?</t>
   </si>
 </sst>
 </file>
@@ -209,13 +197,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -530,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -567,7 +556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -583,11 +572,11 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -603,13 +592,13 @@
       <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -624,12 +613,12 @@
         <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -644,7 +633,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
@@ -667,124 +656,104 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>